<commit_message>
Revu et implémentation des specifications lié à l'apparition des créatures / le scoring. Modification du sort explosion pour qu'il puisse toucher plusieurs cible.
</commit_message>
<xml_diff>
--- a/gamedesign/Specifications.xlsx
+++ b/gamedesign/Specifications.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="Scoring" sheetId="1" r:id="rId1"/>
     <sheet name="Feedback" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="Courbe d'apparition ennemis" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
   <si>
     <t>SCORE</t>
   </si>
@@ -24,9 +24,6 @@
     <t>PLAYER</t>
   </si>
   <si>
-    <t>LIFE</t>
-  </si>
-  <si>
     <t>ENNEMIS PRESENTS DANS L'ARENE</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>Valeur</t>
   </si>
   <si>
-    <t>Score gagner pour le skill de l'ennemi</t>
-  </si>
-  <si>
     <t>Gagner un cœur</t>
   </si>
   <si>
@@ -175,6 +169,36 @@
   </si>
   <si>
     <t>SCORE POUR ENNEMI MARRON</t>
+  </si>
+  <si>
+    <t>COEFFICIENT DE DIFFICULTE</t>
+  </si>
+  <si>
+    <t>POINTS DE VIE</t>
+  </si>
+  <si>
+    <t>DUREE DE LA PARTIE</t>
+  </si>
+  <si>
+    <t>Nombre de créatures maximum dans l'arène</t>
+  </si>
+  <si>
+    <t>Intervalle d'apparition des créatures</t>
+  </si>
+  <si>
+    <t>NOMBRES DE CREATURES DANS L'ARENE</t>
+  </si>
+  <si>
+    <t>INTERVALLE INITIAL</t>
+  </si>
+  <si>
+    <t>Score gagner pour le kill de l'ennemi</t>
+  </si>
+  <si>
+    <t>B3*((MOYENNE(C3:C4)/G2)*B5)</t>
+  </si>
+  <si>
+    <t>B4*((MOYENNE(C3:C4)/G2)*B5)</t>
   </si>
 </sst>
 </file>
@@ -565,13 +589,14 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -583,16 +608,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -600,24 +625,24 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -625,20 +650,26 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1">
-        <f>B3*(AVERAGE(C3:C4)/G2)</f>
-        <v>3.333333333333333</v>
+        <f>B3*((AVERAGE(C3:C4)/G2))</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1">
-        <f>B4*(AVERAGE(C3:C4)/G2)</f>
-        <v>1.6666666666666665</v>
+        <f>B4*((AVERAGE(C3:C4)/G2))</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -652,7 +683,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,299 +697,299 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="C9" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -972,12 +1003,84 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="1">
+        <f>((B2+B3)/B5)/2</f>
+        <v>9.8249999999999993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10">
+        <f>B7- (((B9-B6)+B3)/(10-B4))</f>
+        <v>1.5964285714285715</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout des feedbacks "board"
</commit_message>
<xml_diff>
--- a/gamedesign/Specifications.xlsx
+++ b/gamedesign/Specifications.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
   <si>
     <t>SCORE</t>
   </si>
@@ -691,7 +691,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -883,6 +883,9 @@
       <c r="G8" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="H8" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="10"/>
@@ -921,6 +924,9 @@
       <c r="G10" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="H10" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="30">
       <c r="A11" s="2" t="s">
@@ -941,6 +947,9 @@
       <c r="G11" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="H11" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="30">
       <c r="A12" s="2" t="s">
@@ -960,6 +969,9 @@
       </c>
       <c r="G12" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8">

</xml_diff>